<commit_message>
PostMortem agregado y modificacion de documento Control de Riesgos
</commit_message>
<xml_diff>
--- a/Documentacion/Revision Lanzamiento/Documentacion Los_PRO/R7-ControlRiesgos.xlsx
+++ b/Documentacion/Revision Lanzamiento/Documentacion Los_PRO/R7-ControlRiesgos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aracely Triana\Desktop\NOVENO SEMESTRE\TSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aracely Triana\Documents\GitHub\Gestion_de_titulacion_integral\Documentacion\Revision Lanzamiento\Documentacion Los_PRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BD4D6-0476-4E0C-86A6-BE57B73E3909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6309830-A4AA-4801-8C75-7908979B660A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t># Riesgo</t>
   </si>
@@ -895,8 +896,8 @@
   </sheetPr>
   <dimension ref="A4:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -978,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="10">
-        <f>D11*C11</f>
+        <f t="shared" ref="E11:E22" si="0">D11*C11</f>
         <v>9</v>
       </c>
       <c r="F11" s="20" t="s">
@@ -987,8 +988,12 @@
       <c r="G11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="5">
+        <v>43808</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="J11" s="6" t="s">
         <v>49</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="10">
-        <f>D12*C12</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -1019,8 +1024,12 @@
       <c r="G12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="5">
+        <v>43809</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="J12" s="6" t="s">
         <v>50</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="10">
-        <f>D13*C13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F13" s="12" t="s">
@@ -1051,8 +1060,12 @@
       <c r="G13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
+      <c r="H13" s="5">
+        <v>43810</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="J13" s="6" t="s">
         <v>51</v>
       </c>
@@ -1074,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="10">
-        <f>D14*C14</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F14" s="12" t="s">
@@ -1083,8 +1096,12 @@
       <c r="G14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
+      <c r="H14" s="5">
+        <v>43811</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="J14" s="6" t="s">
         <v>52</v>
       </c>
@@ -1103,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="10">
-        <f>D15*C15</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F15" s="12"/>
@@ -1126,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="10">
-        <f>D16*C16</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F16" s="18"/>
@@ -1135,7 +1152,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>5</v>
       </c>
@@ -1149,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="10">
-        <f>D17*C17</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F17" s="10"/>
@@ -1172,7 +1189,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="10">
-        <f>D18*C18</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F18" s="18"/>
@@ -1195,7 +1212,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="10">
-        <f>D19*C19</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F19" s="18"/>
@@ -1218,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="10">
-        <f>D20*C20</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F20" s="18"/>
@@ -1233,7 +1250,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="10">
-        <f>D21*C21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" s="18"/>
@@ -1248,7 +1265,7 @@
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="10">
-        <f>D22*C22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="18"/>

</xml_diff>